<commit_message>
Converted worksheets into excel table
</commit_message>
<xml_diff>
--- a/Continental Death counts.xlsx
+++ b/Continental Death counts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\waith\OneDrive\Documents\GitHub\Covid19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{686A03CE-D0DC-4DC3-85E9-3A701D8EC51E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6494376C-9DF7-4BF1-8D66-A83BB8FA1FE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -101,6 +101,17 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D571FC25-A7CA-47CE-A843-816E4BB01511}" name="Table1" displayName="Table1" ref="A1:B1048576" totalsRowShown="0">
+  <autoFilter ref="A1:B1048576" xr:uid="{D571FC25-A7CA-47CE-A843-816E4BB01511}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{D90306B6-2BB5-4240-9987-BDA629CC00F3}" name="continent"/>
+    <tableColumn id="2" xr3:uid="{4558F5F5-A707-476E-9065-376C52AC3147}" name="HighestDeathCount"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -403,13 +414,13 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -470,5 +481,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>